<commit_message>
Got the yellper to communicate with the excel imput.
</commit_message>
<xml_diff>
--- a/src/Yelpreviews.xlsx
+++ b/src/Yelpreviews.xlsx
@@ -3,7 +3,7 @@
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
-    <s:workbookView activeTab="2"/>
+    <s:workbookView activeTab="11"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="392" sheetId="1" r:id="rId1"/>
@@ -3914,8 +3914,8 @@
     <col customWidth="1" max="1" min="1" style="21" width="11.83203125"/>
     <col customWidth="1" max="2" min="2" style="21" width="15.1640625"/>
     <col customWidth="1" max="3" min="3" style="21" width="100.5"/>
-    <col customWidth="1" max="9" min="4" style="21" width="8.83203125"/>
-    <col customWidth="1" max="16384" min="10" style="21" width="8.83203125"/>
+    <col customWidth="1" max="10" min="4" style="21" width="8.83203125"/>
+    <col customWidth="1" max="16384" min="11" style="21" width="8.83203125"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="30" r="1" spans="1:3">
@@ -3923,7 +3923,6 @@
         <v>411</v>
       </c>
     </row>
-    <row r="2" spans="1:3"/>
     <row r="3" spans="1:3">
       <c r="A3" s="19" t="s">
         <v>2</v>
@@ -4089,8 +4088,8 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9476,7 +9475,7 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>

</xml_diff>